<commit_message>
Added Voucher Excel Upload Feature
</commit_message>
<xml_diff>
--- a/assets/uploads/testbook.xlsx
+++ b/assets/uploads/testbook.xlsx
@@ -27,93 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Opportunity Title</t>
+    <t>Voucher Code</t>
   </si>
   <si>
-    <t>Purpose</t>
+    <t>Gyxwyzx123</t>
   </si>
   <si>
-    <t>Eligibility</t>
-  </si>
-  <si>
-    <t>Level Of Study</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Value in dollars</t>
-  </si>
-  <si>
-    <t>Course</t>
-  </si>
-  <si>
-    <t>Country Of Study</t>
-  </si>
-  <si>
-    <t>Deadline</t>
-  </si>
-  <si>
-    <t>WebLink</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>To Kill Peepul</t>
-  </si>
-  <si>
-    <t>Assasins</t>
-  </si>
-  <si>
-    <t>300Level</t>
-  </si>
-  <si>
-    <t>Assasination</t>
-  </si>
-  <si>
-    <t>Nigeria :)</t>
-  </si>
-  <si>
-    <t>Today</t>
-  </si>
-  <si>
-    <t>http://lawrencetalks.com</t>
-  </si>
-  <si>
-    <t>Grant</t>
-  </si>
-  <si>
-    <t>Some random opportunity</t>
-  </si>
-  <si>
-    <t>£50,000</t>
-  </si>
-  <si>
-    <t>Some random opportunity2</t>
-  </si>
-  <si>
-    <t>To Kill Peepul :)</t>
-  </si>
-  <si>
-    <t>500Level</t>
-  </si>
-  <si>
-    <t>£70,000</t>
-  </si>
-  <si>
-    <t>Uk :)</t>
-  </si>
-  <si>
-    <t>6th February 2017</t>
-  </si>
-  <si>
-    <t>Competition</t>
-  </si>
-  <si>
-    <t>Datecreated</t>
+    <t>Vwyx55rXLt</t>
   </si>
 </sst>
 </file>
@@ -476,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,119 +420,27 @@
     <col min="12" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="1"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1">
-        <v>60000</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3">
-        <v>80000</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" t="s">
-        <v>27</v>
-      </c>
+      <c r="E3" s="4"/>
+      <c r="J3" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed expire button on posts
</commit_message>
<xml_diff>
--- a/assets/uploads/testbook.xlsx
+++ b/assets/uploads/testbook.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lawrence Agbani\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lawrence Agbani\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14325" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14325" windowHeight="7410"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,15 +27,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Voucher Code</t>
-  </si>
-  <si>
-    <t>Gyxwyzx123</t>
-  </si>
-  <si>
-    <t>Vwyx55rXLt</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+  <si>
+    <t>Opportunity Title</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Eligibility</t>
+  </si>
+  <si>
+    <t>Level Of Study</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Value in dollars</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Country Of Study</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>WebLink</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>To Kill Peepul</t>
+  </si>
+  <si>
+    <t>Assasins</t>
+  </si>
+  <si>
+    <t>300Level</t>
+  </si>
+  <si>
+    <t>Assasination</t>
+  </si>
+  <si>
+    <t>Nigeria :)</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>http://lawrencetalks.com</t>
+  </si>
+  <si>
+    <t>Some random opportunity</t>
+  </si>
+  <si>
+    <t>£50,000</t>
+  </si>
+  <si>
+    <t>Some random opportunity2</t>
+  </si>
+  <si>
+    <t>To Kill Peepul :)</t>
+  </si>
+  <si>
+    <t>500Level</t>
+  </si>
+  <si>
+    <t>£70,000</t>
+  </si>
+  <si>
+    <t>Uk :)</t>
+  </si>
+  <si>
+    <t>6th February 2017</t>
+  </si>
+  <si>
+    <t>Datecreated</t>
+  </si>
+  <si>
+    <t>Bachelor</t>
+  </si>
+  <si>
+    <t>Master</t>
   </si>
 </sst>
 </file>
@@ -211,6 +289,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -246,6 +341,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -398,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,27 +532,119 @@
     <col min="12" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="1"/>
-      <c r="J2" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1">
+        <v>60000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="J3" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3">
+        <v>80000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>